<commit_message>
Adding some for loops and file system intergration
</commit_message>
<xml_diff>
--- a/Outbox/Output.xlsx
+++ b/Outbox/Output.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1065,7 +1066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -1202,11 +1203,6 @@
     <row r="6">
       <c r="A6" t="n">
         <v>22356568</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>34256354</v>
       </c>
     </row>
   </sheetData>
@@ -1377,4 +1373,151 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
+  <cols>
+    <col width="18.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="18.140625" customWidth="1" style="11" min="2" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dummy template </t>
+        </is>
+      </c>
+      <c r="B1" s="12" t="n"/>
+      <c r="C1" s="12" t="n"/>
+      <c r="D1" s="12" t="n"/>
+      <c r="E1" s="12" t="n"/>
+      <c r="F1" s="12" t="n"/>
+    </row>
+    <row r="2" ht="75" customHeight="1" s="11">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Part number of product. This number must be unique.</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> End user (customer) specific part number or product ID.</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The minimum order quantity for the product based on the Unit Of Measure.</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Number of working days required to deliver the product (ARO).</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Price of Product.  Do not use any signs or commas.</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cost Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>40 Max Length</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>40 Max Length</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>1 to 50000</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>1 to 999</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>0.00 to 10000000.00</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>0.00 to 10000000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Required</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr"/>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="7" t="inlineStr"/>
+      <c r="F4" s="9" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Part Number</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>NSN Number</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Minimum Order Quantity</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Delivery Time</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>Final Price</t>
+        </is>
+      </c>
+      <c r="F5" s="9" t="inlineStr">
+        <is>
+          <t>Cost Price</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working with on import and one sheet
</commit_message>
<xml_diff>
--- a/Outbox/Output.xlsx
+++ b/Outbox/Output.xlsx
@@ -1204,117 +1204,126 @@
       <c r="A6" t="n">
         <v>22356568</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C6" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>112.17</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>34256354</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C7" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>200</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>44637355</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C8" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>114.2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>74.23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>55261434</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C9" t="n">
-        <v>22691</v>
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>27.67</v>
+      </c>
+      <c r="F9" t="n">
+        <v>18.56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>66464788</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C10" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>505</v>
+      </c>
+      <c r="F10" t="n">
+        <v>411.14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>77423423</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C11" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>800</v>
+      </c>
+      <c r="F11" t="n">
+        <v>118.84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>88888856</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C12" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20.96</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>94757647</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C13" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>812.01</v>
+      </c>
+      <c r="F13" t="n">
+        <v>682.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>10342423</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Rnd Manufacturer</t>
-        </is>
-      </c>
       <c r="C14" t="n">
-        <v>22691</v>
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>28.68</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on adding file switching
</commit_message>
<xml_diff>
--- a/Outbox/Output.xlsx
+++ b/Outbox/Output.xlsx
@@ -8,7 +8,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1480,151 +1479,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12"/>
-  <cols>
-    <col width="18.140625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="18.140625" customWidth="1" style="11" min="2" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Dummy template </t>
-        </is>
-      </c>
-      <c r="B1" s="12" t="n"/>
-      <c r="C1" s="12" t="n"/>
-      <c r="D1" s="12" t="n"/>
-      <c r="E1" s="12" t="n"/>
-      <c r="F1" s="12" t="n"/>
-    </row>
-    <row r="2" ht="75" customHeight="1" s="11">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Part number of product. This number must be unique.</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> End user (customer) specific part number or product ID.</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The minimum order quantity for the product based on the Unit Of Measure.</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Number of working days required to deliver the product (ARO).</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Price of Product.  Do not use any signs or commas.</t>
-        </is>
-      </c>
-      <c r="F2" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Cost Price</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>40 Max Length</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>40 Max Length</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>1 to 50000</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>1 to 999</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>0.00 to 10000000.00</t>
-        </is>
-      </c>
-      <c r="F3" s="9" t="inlineStr">
-        <is>
-          <t>0.00 to 10000000.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Required</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr"/>
-      <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr"/>
-      <c r="E4" s="7" t="inlineStr"/>
-      <c r="F4" s="9" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>NSN Number</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>Minimum Order Quantity</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>Delivery Time</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>Final Price</t>
-        </is>
-      </c>
-      <c r="F5" s="9" t="inlineStr">
-        <is>
-          <t>Cost Price</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished File switching functionality
</commit_message>
<xml_diff>
--- a/Outbox/Output.xlsx
+++ b/Outbox/Output.xlsx
@@ -1340,7 +1340,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1472,6 +1472,132 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>22356568</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>112.17</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>34256354</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>200</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>44637355</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>114.2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>74.23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>55261434</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>27.67</v>
+      </c>
+      <c r="F9" t="n">
+        <v>18.56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>66464788</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>505</v>
+      </c>
+      <c r="F10" t="n">
+        <v>411.14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>77423423</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>800</v>
+      </c>
+      <c r="F11" t="n">
+        <v>118.84</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>88888856</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20.96</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>94757647</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>812.01</v>
+      </c>
+      <c r="F13" t="n">
+        <v>682.09</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10342423</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>28.68</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>